<commit_message>
Movebanks and abilities work for the minor legends
</commit_message>
<xml_diff>
--- a/stuff/pokemon game.xlsx
+++ b/stuff/pokemon game.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git\PokemonXhenos\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8662B4-9C67-4667-BAE7-D350C23DB52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A40537B-5722-42CA-A098-78563B4DB0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12825" windowWidth="16440" windowHeight="28320" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3199" uniqueCount="1663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3209" uniqueCount="1672">
   <si>
     <t>Leafer</t>
   </si>
@@ -5025,6 +5025,33 @@
   </si>
   <si>
     <t>Fable Stone</t>
+  </si>
+  <si>
+    <t>Ryder</t>
+  </si>
+  <si>
+    <t>2. Blohadel</t>
+  </si>
+  <si>
+    <t>3. Flamigo</t>
+  </si>
+  <si>
+    <t>5. Necrozma</t>
+  </si>
+  <si>
+    <t>6. Alakazam</t>
+  </si>
+  <si>
+    <t>Galactic -&gt; Dark/Galactic</t>
+  </si>
+  <si>
+    <t>4. Superchargo</t>
+  </si>
+  <si>
+    <t>1. Icy Serpent</t>
+  </si>
+  <si>
+    <t>Icy Serpent: Dragon Dance/Sword of Dawn/Ice Spinner/Earthquake/Magic Fang/Magic Reflect</t>
   </si>
 </sst>
 </file>
@@ -6062,8 +6089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO33" sqref="AO33"/>
+    <sheetView tabSelected="1" topLeftCell="F28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8238,6 +8265,9 @@
       <c r="Q33" s="33" t="s">
         <v>186</v>
       </c>
+      <c r="S33" s="33" t="s">
+        <v>1663</v>
+      </c>
       <c r="U33" t="s">
         <v>206</v>
       </c>
@@ -8329,6 +8359,9 @@
       <c r="Q34" t="s">
         <v>1571</v>
       </c>
+      <c r="S34" t="s">
+        <v>1670</v>
+      </c>
       <c r="U34" t="s">
         <v>208</v>
       </c>
@@ -8417,6 +8450,9 @@
       <c r="Q35" t="s">
         <v>1109</v>
       </c>
+      <c r="S35" t="s">
+        <v>1664</v>
+      </c>
       <c r="U35" t="s">
         <v>210</v>
       </c>
@@ -8505,6 +8541,9 @@
       <c r="Q36" t="s">
         <v>1110</v>
       </c>
+      <c r="S36" t="s">
+        <v>1665</v>
+      </c>
       <c r="U36" t="s">
         <v>212</v>
       </c>
@@ -8593,6 +8632,9 @@
       <c r="Q37" t="s">
         <v>1111</v>
       </c>
+      <c r="S37" t="s">
+        <v>1669</v>
+      </c>
       <c r="X37" s="11" t="s">
         <v>176</v>
       </c>
@@ -8678,6 +8720,12 @@
       <c r="Q38" t="s">
         <v>1112</v>
       </c>
+      <c r="S38" t="s">
+        <v>1666</v>
+      </c>
+      <c r="T38" t="s">
+        <v>1668</v>
+      </c>
       <c r="X38" t="s">
         <v>214</v>
       </c>
@@ -8763,6 +8811,9 @@
       <c r="Q39" t="s">
         <v>1113</v>
       </c>
+      <c r="S39" t="s">
+        <v>1667</v>
+      </c>
       <c r="X39" t="s">
         <v>215</v>
       </c>
@@ -8836,6 +8887,9 @@
       <c r="K40">
         <v>399</v>
       </c>
+      <c r="N40" t="s">
+        <v>1658</v>
+      </c>
       <c r="O40" t="s">
         <v>1085</v>
       </c>
@@ -8844,6 +8898,9 @@
       </c>
       <c r="Q40" t="s">
         <v>1114</v>
+      </c>
+      <c r="S40" t="s">
+        <v>1671</v>
       </c>
       <c r="X40" s="10" t="s">
         <v>216</v>

</xml_diff>

<commit_message>
Bug fixes and e4 split map work!
</commit_message>
<xml_diff>
--- a/stuff/pokemon game.xlsx
+++ b/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git\PokemonXhenos\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A40537B-5722-42CA-A098-78563B4DB0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC8B703-1874-4CD0-B367-3F3D92BB25B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3209" uniqueCount="1672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3210" uniqueCount="1673">
   <si>
     <t>Leafer</t>
   </si>
@@ -5052,6 +5052,9 @@
   </si>
   <si>
     <t>Icy Serpent: Dragon Dance/Sword of Dawn/Ice Spinner/Earthquake/Magic Fang/Magic Reflect</t>
+  </si>
+  <si>
+    <t>Move Encyclopedia</t>
   </si>
 </sst>
 </file>
@@ -5775,10 +5778,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CCCD70F4-8B57-40C5-9200-528EDFFF7692}" name="Table5" displayName="Table5" ref="AK29:AN426" totalsRowShown="0">
-  <autoFilter ref="AK29:AN426" xr:uid="{CCCD70F4-8B57-40C5-9200-528EDFFF7692}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AK30:AN426">
-    <sortCondition ref="AM29:AM426"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CCCD70F4-8B57-40C5-9200-528EDFFF7692}" name="Table5" displayName="Table5" ref="AK29:AN427" totalsRowShown="0">
+  <autoFilter ref="AK29:AN427" xr:uid="{CCCD70F4-8B57-40C5-9200-528EDFFF7692}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AK30:AN427">
+    <sortCondition ref="AM29:AM427"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{26A53F18-86E2-4791-9F01-3774B056CCDA}" name="Pos"/>
@@ -6089,8 +6092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+    <sheetView tabSelected="1" topLeftCell="Q136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ141" sqref="AJ141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15554,7 +15557,7 @@
         <v>301</v>
       </c>
       <c r="AL122" t="s">
-        <v>1381</v>
+        <v>1672</v>
       </c>
       <c r="AM122">
         <v>0</v>
@@ -15624,10 +15627,10 @@
         <v>1.4E-3</v>
       </c>
       <c r="AK123">
-        <v>333</v>
+        <v>302</v>
       </c>
       <c r="AL123" t="s">
-        <v>1351</v>
+        <v>1381</v>
       </c>
       <c r="AM123">
         <v>0</v>
@@ -15697,16 +15700,13 @@
         <v>1.4E-3</v>
       </c>
       <c r="AK124">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="AL124" t="s">
-        <v>1266</v>
+        <v>1351</v>
       </c>
       <c r="AM124">
         <v>0</v>
-      </c>
-      <c r="AN124" t="s">
-        <v>1563</v>
       </c>
     </row>
     <row r="125" spans="2:40" x14ac:dyDescent="0.25">
@@ -15773,13 +15773,16 @@
         <v>1.4E-3</v>
       </c>
       <c r="AK125">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="AL125" t="s">
-        <v>1415</v>
+        <v>1266</v>
       </c>
       <c r="AM125">
         <v>0</v>
+      </c>
+      <c r="AN125" t="s">
+        <v>1563</v>
       </c>
     </row>
     <row r="126" spans="2:40" x14ac:dyDescent="0.25">
@@ -15849,7 +15852,7 @@
         <v>355</v>
       </c>
       <c r="AL126" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="AM126">
         <v>0</v>
@@ -15922,7 +15925,7 @@
         <v>356</v>
       </c>
       <c r="AL127" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="AM127">
         <v>0</v>
@@ -15995,7 +15998,7 @@
         <v>357</v>
       </c>
       <c r="AL128" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="AM128">
         <v>0</v>
@@ -16068,7 +16071,7 @@
         <v>358</v>
       </c>
       <c r="AL129" t="s">
-        <v>1472</v>
+        <v>1418</v>
       </c>
       <c r="AM129">
         <v>0</v>
@@ -16141,7 +16144,7 @@
         <v>359</v>
       </c>
       <c r="AL130" t="s">
-        <v>1388</v>
+        <v>1472</v>
       </c>
       <c r="AM130">
         <v>0</v>
@@ -16214,7 +16217,7 @@
         <v>360</v>
       </c>
       <c r="AL131" t="s">
-        <v>1474</v>
+        <v>1388</v>
       </c>
       <c r="AM131">
         <v>0</v>
@@ -16287,7 +16290,7 @@
         <v>361</v>
       </c>
       <c r="AL132" t="s">
-        <v>1471</v>
+        <v>1474</v>
       </c>
       <c r="AM132">
         <v>0</v>
@@ -16360,7 +16363,7 @@
         <v>362</v>
       </c>
       <c r="AL133" t="s">
-        <v>1403</v>
+        <v>1471</v>
       </c>
       <c r="AM133">
         <v>0</v>
@@ -16433,7 +16436,7 @@
         <v>363</v>
       </c>
       <c r="AL134" t="s">
-        <v>1394</v>
+        <v>1403</v>
       </c>
       <c r="AM134">
         <v>0</v>
@@ -16503,10 +16506,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK135">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AL135" t="s">
-        <v>1408</v>
+        <v>1394</v>
       </c>
       <c r="AM135">
         <v>0</v>
@@ -16576,10 +16579,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK136">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AL136" t="s">
-        <v>1387</v>
+        <v>1408</v>
       </c>
       <c r="AM136">
         <v>0</v>
@@ -16648,8 +16651,11 @@
       <c r="AI137" s="35">
         <v>2.0999999999999999E-3</v>
       </c>
+      <c r="AK137">
+        <v>369</v>
+      </c>
       <c r="AL137" t="s">
-        <v>1641</v>
+        <v>1387</v>
       </c>
       <c r="AM137">
         <v>0</v>
@@ -16722,7 +16728,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AL138" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="AM138">
         <v>0</v>
@@ -16792,7 +16798,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AL139" t="s">
-        <v>1651</v>
+        <v>1642</v>
       </c>
       <c r="AM139">
         <v>0</v>
@@ -16862,7 +16868,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AL140" t="s">
-        <v>1662</v>
+        <v>1651</v>
       </c>
       <c r="AM140">
         <v>0</v>
@@ -16938,14 +16944,11 @@
       <c r="AI141" s="35">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="AK141">
-        <v>73</v>
-      </c>
       <c r="AL141" t="s">
-        <v>1271</v>
+        <v>1662</v>
       </c>
       <c r="AM141">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="2:39" x14ac:dyDescent="0.25">
@@ -17022,10 +17025,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK142">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AL142" t="s">
-        <v>1228</v>
+        <v>1271</v>
       </c>
       <c r="AM142">
         <v>1</v>
@@ -17102,10 +17105,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK143">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL143" t="s">
-        <v>1367</v>
+        <v>1228</v>
       </c>
       <c r="AM143">
         <v>1</v>
@@ -17194,10 +17197,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK144">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AL144" t="s">
-        <v>1281</v>
+        <v>1367</v>
       </c>
       <c r="AM144">
         <v>1</v>
@@ -17279,10 +17282,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK145">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AL145" t="s">
-        <v>1233</v>
+        <v>1281</v>
       </c>
       <c r="AM145">
         <v>1</v>
@@ -17389,10 +17392,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK146">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AL146" t="s">
-        <v>881</v>
+        <v>1233</v>
       </c>
       <c r="AM146">
         <v>1</v>
@@ -17496,10 +17499,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK147">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AL147" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="AM147">
         <v>1</v>
@@ -17603,10 +17606,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK148">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AL148" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="AM148">
         <v>1</v>
@@ -17710,10 +17713,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK149">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AL149" t="s">
-        <v>897</v>
+        <v>883</v>
       </c>
       <c r="AM149">
         <v>1</v>
@@ -17817,16 +17820,13 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK150">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AL150" t="s">
-        <v>879</v>
+        <v>897</v>
       </c>
       <c r="AM150">
         <v>1</v>
-      </c>
-      <c r="AN150" t="s">
-        <v>1563</v>
       </c>
     </row>
     <row r="151" spans="1:40" x14ac:dyDescent="0.25">
@@ -17924,10 +17924,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK151">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AL151" t="s">
-        <v>891</v>
+        <v>879</v>
       </c>
       <c r="AM151">
         <v>1</v>
@@ -18037,13 +18037,16 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK152">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AL152" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="AM152">
         <v>1</v>
+      </c>
+      <c r="AN152" t="s">
+        <v>1563</v>
       </c>
     </row>
     <row r="153" spans="1:40" x14ac:dyDescent="0.25">
@@ -18144,10 +18147,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK153">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AL153" t="s">
-        <v>1640</v>
+        <v>890</v>
       </c>
       <c r="AM153">
         <v>1</v>
@@ -18248,10 +18251,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK154">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AL154" t="s">
-        <v>886</v>
+        <v>1640</v>
       </c>
       <c r="AM154">
         <v>1</v>
@@ -18355,10 +18358,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK155">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AL155" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="AM155">
         <v>1</v>
@@ -18462,10 +18465,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK156">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AL156" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="AM156">
         <v>1</v>
@@ -18569,10 +18572,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK157">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AL157" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="AM157">
         <v>1</v>
@@ -18676,10 +18679,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK158">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AL158" t="s">
-        <v>878</v>
+        <v>889</v>
       </c>
       <c r="AM158">
         <v>1</v>
@@ -18783,10 +18786,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK159">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AL159" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="AM159">
         <v>1</v>
@@ -18887,10 +18890,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK160">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AL160" t="s">
-        <v>892</v>
+        <v>880</v>
       </c>
       <c r="AM160">
         <v>1</v>
@@ -18994,16 +18997,13 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK161">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AL161" t="s">
-        <v>1476</v>
+        <v>892</v>
       </c>
       <c r="AM161">
         <v>1</v>
-      </c>
-      <c r="AN161" t="s">
-        <v>1563</v>
       </c>
     </row>
     <row r="162" spans="1:40" x14ac:dyDescent="0.25">
@@ -19104,13 +19104,16 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK162">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AL162" t="s">
-        <v>988</v>
+        <v>1476</v>
       </c>
       <c r="AM162">
         <v>1</v>
+      </c>
+      <c r="AN162" t="s">
+        <v>1563</v>
       </c>
     </row>
     <row r="163" spans="1:40" x14ac:dyDescent="0.25">
@@ -19211,10 +19214,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK163">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AL163" t="s">
-        <v>1477</v>
+        <v>988</v>
       </c>
       <c r="AM163">
         <v>1</v>
@@ -19321,10 +19324,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK164">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AL164" t="s">
-        <v>898</v>
+        <v>1477</v>
       </c>
       <c r="AM164">
         <v>1</v>
@@ -19428,10 +19431,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK165">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AL165" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="AM165">
         <v>1</v>
@@ -19532,16 +19535,13 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK166">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AL166" t="s">
-        <v>1643</v>
+        <v>906</v>
       </c>
       <c r="AM166">
         <v>1</v>
-      </c>
-      <c r="AN166" t="s">
-        <v>1563</v>
       </c>
     </row>
     <row r="167" spans="1:40" x14ac:dyDescent="0.25">
@@ -19640,10 +19640,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK167">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AL167" t="s">
-        <v>904</v>
+        <v>1643</v>
       </c>
       <c r="AM167">
         <v>1</v>
@@ -19748,13 +19748,16 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK168">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AL168" t="s">
-        <v>1478</v>
+        <v>904</v>
       </c>
       <c r="AM168">
         <v>1</v>
+      </c>
+      <c r="AN168" t="s">
+        <v>1563</v>
       </c>
     </row>
     <row r="169" spans="1:40" x14ac:dyDescent="0.25">
@@ -19852,10 +19855,10 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="AK169">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AL169" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="AM169">
         <v>1</v>
@@ -19959,10 +19962,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK170">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AL170" t="s">
-        <v>899</v>
+        <v>1479</v>
       </c>
       <c r="AM170">
         <v>1</v>
@@ -20064,10 +20067,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK171">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AL171" t="s">
-        <v>1014</v>
+        <v>899</v>
       </c>
       <c r="AM171">
         <v>1</v>
@@ -20169,10 +20172,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK172">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AL172" t="s">
-        <v>903</v>
+        <v>1014</v>
       </c>
       <c r="AM172">
         <v>1</v>
@@ -20268,10 +20271,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK173">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AL173" t="s">
-        <v>909</v>
+        <v>903</v>
       </c>
       <c r="AM173">
         <v>1</v>
@@ -20372,10 +20375,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK174">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AL174" t="s">
-        <v>1481</v>
+        <v>909</v>
       </c>
       <c r="AM174">
         <v>1</v>
@@ -20476,10 +20479,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK175">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL175" t="s">
-        <v>902</v>
+        <v>1481</v>
       </c>
       <c r="AM175">
         <v>1</v>
@@ -20577,10 +20580,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK176">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AL176" t="s">
-        <v>1015</v>
+        <v>902</v>
       </c>
       <c r="AM176">
         <v>1</v>
@@ -20679,10 +20682,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK177">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AL177" t="s">
-        <v>884</v>
+        <v>1015</v>
       </c>
       <c r="AM177">
         <v>1</v>
@@ -20781,10 +20784,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK178">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AL178" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="AM178">
         <v>1</v>
@@ -20880,10 +20883,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK179">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AL179" t="s">
-        <v>1366</v>
+        <v>885</v>
       </c>
       <c r="AM179">
         <v>1</v>
@@ -20982,10 +20985,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK180">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AL180" t="s">
-        <v>895</v>
+        <v>1366</v>
       </c>
       <c r="AM180">
         <v>1</v>
@@ -21084,10 +21087,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK181">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AL181" t="s">
-        <v>1238</v>
+        <v>895</v>
       </c>
       <c r="AM181">
         <v>1</v>
@@ -21183,10 +21186,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK182">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AL182" t="s">
-        <v>1250</v>
+        <v>1238</v>
       </c>
       <c r="AM182">
         <v>1</v>
@@ -21284,16 +21287,13 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK183">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AL183" t="s">
-        <v>1060</v>
+        <v>1250</v>
       </c>
       <c r="AM183">
         <v>1</v>
-      </c>
-      <c r="AN183" t="s">
-        <v>1564</v>
       </c>
     </row>
     <row r="184" spans="1:40" x14ac:dyDescent="0.25">
@@ -21394,13 +21394,16 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK184">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AL184" t="s">
-        <v>900</v>
+        <v>1060</v>
       </c>
       <c r="AM184">
         <v>1</v>
+      </c>
+      <c r="AN184" t="s">
+        <v>1564</v>
       </c>
     </row>
     <row r="185" spans="1:40" x14ac:dyDescent="0.25">
@@ -21498,10 +21501,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK185">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AL185" t="s">
-        <v>910</v>
+        <v>900</v>
       </c>
       <c r="AM185">
         <v>1</v>
@@ -21602,10 +21605,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK186">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AL186" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="AM186">
         <v>1</v>
@@ -21706,10 +21709,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK187">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AL187" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="AM187">
         <v>1</v>
@@ -21807,10 +21810,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK188">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL188" t="s">
-        <v>928</v>
+        <v>912</v>
       </c>
       <c r="AM188">
         <v>1</v>
@@ -21909,10 +21912,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK189">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AL189" t="s">
-        <v>914</v>
+        <v>928</v>
       </c>
       <c r="AM189">
         <v>1</v>
@@ -22011,16 +22014,13 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK190">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AL190" t="s">
-        <v>929</v>
+        <v>914</v>
       </c>
       <c r="AM190">
         <v>1</v>
-      </c>
-      <c r="AN190" t="s">
-        <v>1564</v>
       </c>
     </row>
     <row r="191" spans="1:40" x14ac:dyDescent="0.25">
@@ -22113,10 +22113,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK191">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AL191" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AM191">
         <v>1</v>
@@ -22211,13 +22211,16 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK192">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AL192" t="s">
-        <v>915</v>
+        <v>930</v>
       </c>
       <c r="AM192">
         <v>1</v>
+      </c>
+      <c r="AN192" t="s">
+        <v>1564</v>
       </c>
     </row>
     <row r="193" spans="1:40" x14ac:dyDescent="0.25">
@@ -22309,10 +22312,10 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK193">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AL193" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="AM193">
         <v>1</v>
@@ -22413,10 +22416,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK194">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AL194" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="AM194">
         <v>1</v>
@@ -22514,10 +22517,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK195">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AL195" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="AM195">
         <v>1</v>
@@ -22618,10 +22621,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK196">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL196" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="AM196">
         <v>1</v>
@@ -22722,10 +22725,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK197">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AL197" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AM197">
         <v>1</v>
@@ -22826,16 +22829,13 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK198">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AL198" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="AM198">
         <v>1</v>
-      </c>
-      <c r="AN198" t="s">
-        <v>1563</v>
       </c>
     </row>
     <row r="199" spans="1:40" x14ac:dyDescent="0.25">
@@ -22930,13 +22930,16 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK199">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AL199" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="AM199">
         <v>1</v>
+      </c>
+      <c r="AN199" t="s">
+        <v>1563</v>
       </c>
     </row>
     <row r="200" spans="1:40" x14ac:dyDescent="0.25">
@@ -23034,10 +23037,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK200">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AL200" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="AM200">
         <v>1</v>
@@ -23135,10 +23138,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK201">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AL201" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="AM201">
         <v>1</v>
@@ -23236,10 +23239,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK202">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AL202" t="s">
-        <v>1538</v>
+        <v>927</v>
       </c>
       <c r="AM202">
         <v>1</v>
@@ -23334,10 +23337,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK203">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AL203" t="s">
-        <v>1348</v>
+        <v>1538</v>
       </c>
       <c r="AM203">
         <v>1</v>
@@ -23435,10 +23438,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK204">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AL204" t="s">
-        <v>1353</v>
+        <v>1348</v>
       </c>
       <c r="AM204">
         <v>1</v>
@@ -23533,10 +23536,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK205">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL205" t="s">
-        <v>1407</v>
+        <v>1353</v>
       </c>
       <c r="AM205">
         <v>1</v>
@@ -23631,10 +23634,10 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="AK206">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AL206" t="s">
-        <v>1483</v>
+        <v>1407</v>
       </c>
       <c r="AM206">
         <v>1</v>
@@ -23732,10 +23735,10 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK207">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AL207" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="AM207">
         <v>1</v>
@@ -23827,10 +23830,10 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK208">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AL208" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="AM208">
         <v>1</v>
@@ -23923,10 +23926,10 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK209">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AL209" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="AM209">
         <v>1</v>
@@ -24016,10 +24019,10 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK210">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AL210" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="AM210">
         <v>1</v>
@@ -24114,16 +24117,13 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK211">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="AL211" t="s">
-        <v>1245</v>
+        <v>1487</v>
       </c>
       <c r="AM211">
         <v>1</v>
-      </c>
-      <c r="AN211" t="s">
-        <v>1565</v>
       </c>
     </row>
     <row r="212" spans="1:40" x14ac:dyDescent="0.25">
@@ -24212,13 +24212,16 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK212">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="AL212" t="s">
-        <v>1543</v>
+        <v>1245</v>
       </c>
       <c r="AM212">
         <v>1</v>
+      </c>
+      <c r="AN212" t="s">
+        <v>1565</v>
       </c>
     </row>
     <row r="213" spans="1:40" x14ac:dyDescent="0.25">
@@ -24310,10 +24313,10 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK213">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AL213" t="s">
-        <v>1283</v>
+        <v>1543</v>
       </c>
       <c r="AM213">
         <v>1</v>
@@ -24408,10 +24411,10 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK214">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AL214" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="AM214">
         <v>1</v>
@@ -24503,16 +24506,13 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK215">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL215" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="AM215">
         <v>1</v>
-      </c>
-      <c r="AN215" t="s">
-        <v>1565</v>
       </c>
     </row>
     <row r="216" spans="1:40" x14ac:dyDescent="0.25">
@@ -24604,16 +24604,16 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK216">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AL216" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="AM216">
         <v>1</v>
       </c>
       <c r="AN216" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="217" spans="1:40" x14ac:dyDescent="0.25">
@@ -24702,10 +24702,10 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK217">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AL217" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="AM217">
         <v>1</v>
@@ -24806,13 +24806,16 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK218">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AL218" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="AM218">
         <v>1</v>
+      </c>
+      <c r="AN218" t="s">
+        <v>1566</v>
       </c>
     </row>
     <row r="219" spans="1:40" x14ac:dyDescent="0.25">
@@ -24904,16 +24907,13 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK219">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AL219" t="s">
-        <v>1431</v>
+        <v>1288</v>
       </c>
       <c r="AM219">
         <v>1</v>
-      </c>
-      <c r="AN219" t="s">
-        <v>1566</v>
       </c>
     </row>
     <row r="220" spans="1:40" x14ac:dyDescent="0.25">
@@ -25005,13 +25005,16 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK220">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AL220" t="s">
-        <v>1289</v>
+        <v>1431</v>
       </c>
       <c r="AM220">
         <v>1</v>
+      </c>
+      <c r="AN220" t="s">
+        <v>1566</v>
       </c>
     </row>
     <row r="221" spans="1:40" x14ac:dyDescent="0.25">
@@ -25103,16 +25106,13 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK221">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AL221" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="AM221">
         <v>1</v>
-      </c>
-      <c r="AN221" t="s">
-        <v>1565</v>
       </c>
     </row>
     <row r="222" spans="1:40" x14ac:dyDescent="0.25">
@@ -25201,16 +25201,16 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK222">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AL222" t="s">
-        <v>1437</v>
+        <v>1290</v>
       </c>
       <c r="AM222">
         <v>1</v>
       </c>
       <c r="AN222" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="223" spans="1:40" x14ac:dyDescent="0.25">
@@ -25305,10 +25305,10 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK223">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AL223" t="s">
-        <v>1291</v>
+        <v>1437</v>
       </c>
       <c r="AM223">
         <v>1</v>
@@ -25403,13 +25403,16 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="AK224">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AL224" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="AM224">
         <v>1</v>
+      </c>
+      <c r="AN224" t="s">
+        <v>1566</v>
       </c>
     </row>
     <row r="225" spans="1:40" x14ac:dyDescent="0.25">
@@ -25501,10 +25504,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK225">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="AL225" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="AM225">
         <v>1</v>
@@ -25596,10 +25599,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK226">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AL226" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AM226">
         <v>1</v>
@@ -25691,10 +25694,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK227">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AL227" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="AM227">
         <v>1</v>
@@ -25789,10 +25792,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK228">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AL228" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="AM228">
         <v>1</v>
@@ -25899,10 +25902,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK229">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AL229" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="AM229">
         <v>1</v>
@@ -26006,10 +26009,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK230">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AL230" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="AM230">
         <v>1</v>
@@ -26113,10 +26116,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK231">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AL231" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="AM231">
         <v>1</v>
@@ -26217,16 +26220,13 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK232">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AL232" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="AM232">
         <v>1</v>
-      </c>
-      <c r="AN232" t="s">
-        <v>1566</v>
       </c>
     </row>
     <row r="233" spans="1:40" x14ac:dyDescent="0.25">
@@ -26327,16 +26327,16 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK233">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AL233" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="AM233">
         <v>1</v>
       </c>
       <c r="AN233" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="234" spans="1:40" x14ac:dyDescent="0.25">
@@ -26434,13 +26434,16 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK234">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AL234" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="AM234">
         <v>1</v>
+      </c>
+      <c r="AN234" t="s">
+        <v>1567</v>
       </c>
     </row>
     <row r="235" spans="1:40" x14ac:dyDescent="0.25">
@@ -26541,16 +26544,13 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK235">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AL235" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="AM235">
         <v>1</v>
-      </c>
-      <c r="AN235" t="s">
-        <v>1566</v>
       </c>
     </row>
     <row r="236" spans="1:40" x14ac:dyDescent="0.25">
@@ -26648,10 +26648,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK236">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AL236" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="AM236">
         <v>1</v>
@@ -26758,10 +26758,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK237">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="AL237" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="AM237">
         <v>1</v>
@@ -26865,10 +26865,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK238">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="AL238" t="s">
-        <v>1546</v>
+        <v>1306</v>
       </c>
       <c r="AM238">
         <v>1</v>
@@ -26975,16 +26975,16 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK239">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="AL239" t="s">
-        <v>1307</v>
+        <v>1546</v>
       </c>
       <c r="AM239">
         <v>1</v>
       </c>
       <c r="AN239" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="240" spans="1:40" x14ac:dyDescent="0.25">
@@ -27085,13 +27085,16 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK240">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AL240" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="AM240">
         <v>1</v>
+      </c>
+      <c r="AN240" t="s">
+        <v>1565</v>
       </c>
     </row>
     <row r="241" spans="1:40" x14ac:dyDescent="0.25">
@@ -27189,10 +27192,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK241">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="AL241" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="AM241">
         <v>1</v>
@@ -27290,16 +27293,13 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK242">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AL242" t="s">
-        <v>1547</v>
+        <v>1309</v>
       </c>
       <c r="AM242">
         <v>1</v>
-      </c>
-      <c r="AN242" t="s">
-        <v>1565</v>
       </c>
     </row>
     <row r="243" spans="1:40" x14ac:dyDescent="0.25">
@@ -27396,13 +27396,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK243">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AL243" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="AM243">
         <v>1</v>
+      </c>
+      <c r="AN243" t="s">
+        <v>1565</v>
       </c>
     </row>
     <row r="244" spans="1:40" x14ac:dyDescent="0.25">
@@ -27498,10 +27501,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK244">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AL244" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="AM244">
         <v>1</v>
@@ -27597,16 +27600,13 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK245">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AL245" t="s">
-        <v>1310</v>
+        <v>1549</v>
       </c>
       <c r="AM245">
         <v>1</v>
-      </c>
-      <c r="AN245" t="s">
-        <v>1566</v>
       </c>
     </row>
     <row r="246" spans="1:40" x14ac:dyDescent="0.25">
@@ -27704,16 +27704,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK246">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AL246" t="s">
-        <v>1550</v>
+        <v>1310</v>
       </c>
       <c r="AM246">
         <v>1</v>
       </c>
       <c r="AN246" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="247" spans="1:40" x14ac:dyDescent="0.25">
@@ -27811,16 +27811,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK247">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AL247" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="AM247">
         <v>1</v>
       </c>
       <c r="AN247" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="248" spans="1:40" x14ac:dyDescent="0.25">
@@ -27915,16 +27915,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK248">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AL248" t="s">
-        <v>1311</v>
+        <v>1551</v>
       </c>
       <c r="AM248">
         <v>1</v>
       </c>
       <c r="AN248" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="249" spans="1:40" x14ac:dyDescent="0.25">
@@ -28025,13 +28025,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK249">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AL249" t="s">
-        <v>1455</v>
+        <v>1311</v>
       </c>
       <c r="AM249">
         <v>1</v>
+      </c>
+      <c r="AN249" t="s">
+        <v>1567</v>
       </c>
     </row>
     <row r="250" spans="1:40" x14ac:dyDescent="0.25">
@@ -28129,16 +28132,13 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK250">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AL250" t="s">
-        <v>1312</v>
+        <v>1455</v>
       </c>
       <c r="AM250">
         <v>1</v>
-      </c>
-      <c r="AN250" t="s">
-        <v>1567</v>
       </c>
     </row>
     <row r="251" spans="1:40" x14ac:dyDescent="0.25">
@@ -28236,13 +28236,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK251">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="AL251" t="s">
-        <v>1553</v>
+        <v>1312</v>
       </c>
       <c r="AM251">
         <v>1</v>
+      </c>
+      <c r="AN251" t="s">
+        <v>1567</v>
       </c>
     </row>
     <row r="252" spans="1:40" x14ac:dyDescent="0.25">
@@ -28337,16 +28340,13 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK252">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AL252" t="s">
-        <v>1313</v>
+        <v>1553</v>
       </c>
       <c r="AM252">
         <v>1</v>
-      </c>
-      <c r="AN252" t="s">
-        <v>1566</v>
       </c>
     </row>
     <row r="253" spans="1:40" x14ac:dyDescent="0.25">
@@ -28433,10 +28433,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK253">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AL253" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="AM253">
         <v>1</v>
@@ -28535,10 +28535,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK254">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AL254" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="AM254">
         <v>1</v>
@@ -28640,13 +28640,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK255">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AL255" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="AM255">
         <v>1</v>
+      </c>
+      <c r="AN255" t="s">
+        <v>1566</v>
       </c>
     </row>
     <row r="256" spans="1:40" x14ac:dyDescent="0.25">
@@ -28744,10 +28747,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK256">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="AL256" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="AM256">
         <v>1</v>
@@ -28848,10 +28851,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK257">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="AL257" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="AM257">
         <v>1</v>
@@ -28949,10 +28952,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK258">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AL258" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="AM258">
         <v>1</v>
@@ -29053,10 +29056,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK259">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AL259" t="s">
-        <v>1554</v>
+        <v>1319</v>
       </c>
       <c r="AM259">
         <v>1</v>
@@ -29157,16 +29160,13 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK260">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AL260" t="s">
-        <v>1320</v>
+        <v>1554</v>
       </c>
       <c r="AM260">
         <v>1</v>
-      </c>
-      <c r="AN260" t="s">
-        <v>1566</v>
       </c>
     </row>
     <row r="261" spans="1:40" x14ac:dyDescent="0.25">
@@ -29261,16 +29261,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK261">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AL261" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="AM261">
         <v>1</v>
       </c>
       <c r="AN261" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="262" spans="1:40" x14ac:dyDescent="0.25">
@@ -29368,16 +29368,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK262">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="AL262" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="AM262">
         <v>1</v>
       </c>
       <c r="AN262" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="263" spans="1:40" x14ac:dyDescent="0.25">
@@ -29475,16 +29475,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK263">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AL263" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="AM263">
         <v>1</v>
       </c>
       <c r="AN263" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="264" spans="1:40" x14ac:dyDescent="0.25">
@@ -29582,10 +29582,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK264">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AL264" t="s">
-        <v>1555</v>
+        <v>1323</v>
       </c>
       <c r="AM264">
         <v>1</v>
@@ -29690,13 +29690,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK265">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AL265" t="s">
-        <v>1324</v>
+        <v>1555</v>
       </c>
       <c r="AM265">
         <v>1</v>
+      </c>
+      <c r="AN265" t="s">
+        <v>1566</v>
       </c>
     </row>
     <row r="266" spans="1:40" x14ac:dyDescent="0.25">
@@ -29795,16 +29798,13 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK266">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="AL266" t="s">
-        <v>1469</v>
+        <v>1324</v>
       </c>
       <c r="AM266">
         <v>1</v>
-      </c>
-      <c r="AN266" t="s">
-        <v>1568</v>
       </c>
     </row>
     <row r="267" spans="1:40" x14ac:dyDescent="0.25">
@@ -29900,13 +29900,16 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK267">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="AL267" t="s">
-        <v>1325</v>
+        <v>1469</v>
       </c>
       <c r="AM267">
         <v>1</v>
+      </c>
+      <c r="AN267" t="s">
+        <v>1568</v>
       </c>
     </row>
     <row r="268" spans="1:40" x14ac:dyDescent="0.25">
@@ -30002,10 +30005,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK268">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AL268" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="AM268">
         <v>1</v>
@@ -30104,10 +30107,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK269">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="AL269" t="s">
-        <v>1219</v>
+        <v>1326</v>
       </c>
       <c r="AM269">
         <v>1</v>
@@ -30209,7 +30212,7 @@
         <v>307</v>
       </c>
       <c r="AL270" t="s">
-        <v>1254</v>
+        <v>1219</v>
       </c>
       <c r="AM270">
         <v>1</v>
@@ -30311,10 +30314,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK271">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AL271" t="s">
-        <v>1252</v>
+        <v>1254</v>
       </c>
       <c r="AM271">
         <v>1</v>
@@ -30404,10 +30407,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK272">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AL272" t="s">
-        <v>1330</v>
+        <v>1252</v>
       </c>
       <c r="AM272">
         <v>1</v>
@@ -30497,7 +30500,7 @@
         <v>313</v>
       </c>
       <c r="AL273" t="s">
-        <v>1278</v>
+        <v>1330</v>
       </c>
       <c r="AM273">
         <v>1</v>
@@ -30590,7 +30593,7 @@
         <v>314</v>
       </c>
       <c r="AL274" t="s">
-        <v>1221</v>
+        <v>1278</v>
       </c>
       <c r="AM274">
         <v>1</v>
@@ -30680,7 +30683,7 @@
         <v>315</v>
       </c>
       <c r="AL275" t="s">
-        <v>1262</v>
+        <v>1221</v>
       </c>
       <c r="AM275">
         <v>1</v>
@@ -30779,7 +30782,7 @@
         <v>316</v>
       </c>
       <c r="AL276" t="s">
-        <v>1232</v>
+        <v>1262</v>
       </c>
       <c r="AM276">
         <v>1</v>
@@ -30881,7 +30884,7 @@
         <v>317</v>
       </c>
       <c r="AL277" t="s">
-        <v>1328</v>
+        <v>1232</v>
       </c>
       <c r="AM277">
         <v>1</v>
@@ -30980,7 +30983,7 @@
         <v>318</v>
       </c>
       <c r="AL278" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="AM278">
         <v>1</v>
@@ -31082,7 +31085,7 @@
         <v>319</v>
       </c>
       <c r="AL279" t="s">
-        <v>1222</v>
+        <v>1329</v>
       </c>
       <c r="AM279">
         <v>1</v>
@@ -31181,7 +31184,7 @@
         <v>320</v>
       </c>
       <c r="AL280" t="s">
-        <v>1414</v>
+        <v>1222</v>
       </c>
       <c r="AM280">
         <v>1</v>
@@ -31280,7 +31283,7 @@
         <v>321</v>
       </c>
       <c r="AL281" t="s">
-        <v>1419</v>
+        <v>1414</v>
       </c>
       <c r="AM281">
         <v>1</v>
@@ -31382,7 +31385,7 @@
         <v>322</v>
       </c>
       <c r="AL282" t="s">
-        <v>1372</v>
+        <v>1419</v>
       </c>
       <c r="AM282">
         <v>1</v>
@@ -31481,7 +31484,7 @@
         <v>323</v>
       </c>
       <c r="AL283" t="s">
-        <v>1363</v>
+        <v>1372</v>
       </c>
       <c r="AM283">
         <v>1</v>
@@ -31582,7 +31585,7 @@
         <v>324</v>
       </c>
       <c r="AL284" t="s">
-        <v>1374</v>
+        <v>1363</v>
       </c>
       <c r="AM284">
         <v>1</v>
@@ -31680,7 +31683,7 @@
         <v>325</v>
       </c>
       <c r="AL285" t="s">
-        <v>1345</v>
+        <v>1374</v>
       </c>
       <c r="AM285">
         <v>1</v>
@@ -31779,7 +31782,7 @@
         <v>326</v>
       </c>
       <c r="AL286" t="s">
-        <v>1405</v>
+        <v>1345</v>
       </c>
       <c r="AM286">
         <v>1</v>
@@ -31875,7 +31878,7 @@
         <v>327</v>
       </c>
       <c r="AL287" t="s">
-        <v>1368</v>
+        <v>1405</v>
       </c>
       <c r="AM287">
         <v>1</v>
@@ -31974,7 +31977,7 @@
         <v>328</v>
       </c>
       <c r="AL288" t="s">
-        <v>1346</v>
+        <v>1368</v>
       </c>
       <c r="AM288">
         <v>1</v>
@@ -32073,7 +32076,7 @@
         <v>329</v>
       </c>
       <c r="AL289" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="AM289">
         <v>1</v>
@@ -32169,7 +32172,7 @@
         <v>330</v>
       </c>
       <c r="AL290" t="s">
-        <v>1370</v>
+        <v>1360</v>
       </c>
       <c r="AM290">
         <v>1</v>
@@ -32268,7 +32271,7 @@
         <v>331</v>
       </c>
       <c r="AL291" t="s">
-        <v>1378</v>
+        <v>1370</v>
       </c>
       <c r="AM291">
         <v>1</v>
@@ -32364,7 +32367,7 @@
         <v>332</v>
       </c>
       <c r="AL292" t="s">
-        <v>1354</v>
+        <v>1378</v>
       </c>
       <c r="AM292">
         <v>1</v>
@@ -32460,10 +32463,10 @@
         <v>6.1999999999999998E-3</v>
       </c>
       <c r="AK293">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AL293" t="s">
-        <v>1347</v>
+        <v>1354</v>
       </c>
       <c r="AM293">
         <v>1</v>
@@ -32559,7 +32562,7 @@
         <v>335</v>
       </c>
       <c r="AL294" t="s">
-        <v>1341</v>
+        <v>1347</v>
       </c>
       <c r="AM294">
         <v>1</v>
@@ -32655,7 +32658,7 @@
         <v>336</v>
       </c>
       <c r="AL295" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
       <c r="AM295">
         <v>1</v>
@@ -32759,7 +32762,7 @@
         <v>337</v>
       </c>
       <c r="AL296" t="s">
-        <v>1364</v>
+        <v>1344</v>
       </c>
       <c r="AM296">
         <v>1</v>
@@ -32860,7 +32863,7 @@
         <v>338</v>
       </c>
       <c r="AL297" t="s">
-        <v>1357</v>
+        <v>1364</v>
       </c>
       <c r="AM297">
         <v>1</v>
@@ -32964,7 +32967,7 @@
         <v>339</v>
       </c>
       <c r="AL298" t="s">
-        <v>1349</v>
+        <v>1357</v>
       </c>
       <c r="AM298">
         <v>1</v>
@@ -33068,7 +33071,7 @@
         <v>340</v>
       </c>
       <c r="AL299" t="s">
-        <v>1253</v>
+        <v>1349</v>
       </c>
       <c r="AM299">
         <v>1</v>
@@ -33169,7 +33172,7 @@
         <v>341</v>
       </c>
       <c r="AL300" t="s">
-        <v>1242</v>
+        <v>1253</v>
       </c>
       <c r="AM300">
         <v>1</v>
@@ -33273,7 +33276,7 @@
         <v>342</v>
       </c>
       <c r="AL301" t="s">
-        <v>1426</v>
+        <v>1242</v>
       </c>
       <c r="AM301">
         <v>1</v>
@@ -33371,10 +33374,10 @@
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="AK302">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AL302" t="s">
-        <v>1218</v>
+        <v>1426</v>
       </c>
       <c r="AM302">
         <v>1</v>
@@ -33481,7 +33484,7 @@
         <v>345</v>
       </c>
       <c r="AL303" t="s">
-        <v>1279</v>
+        <v>1218</v>
       </c>
       <c r="AM303">
         <v>1</v>
@@ -33585,7 +33588,7 @@
         <v>346</v>
       </c>
       <c r="AL304" t="s">
-        <v>1259</v>
+        <v>1279</v>
       </c>
       <c r="AM304">
         <v>1</v>
@@ -33687,7 +33690,7 @@
         <v>347</v>
       </c>
       <c r="AL305" t="s">
-        <v>1557</v>
+        <v>1259</v>
       </c>
       <c r="AM305">
         <v>1</v>
@@ -33789,7 +33792,7 @@
         <v>348</v>
       </c>
       <c r="AL306" t="s">
-        <v>1379</v>
+        <v>1557</v>
       </c>
       <c r="AM306">
         <v>1</v>
@@ -33891,7 +33894,7 @@
         <v>349</v>
       </c>
       <c r="AL307" t="s">
-        <v>1558</v>
+        <v>1379</v>
       </c>
       <c r="AM307">
         <v>1</v>
@@ -33993,7 +33996,7 @@
         <v>350</v>
       </c>
       <c r="AL308" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="AM308">
         <v>1</v>
@@ -34095,7 +34098,7 @@
         <v>351</v>
       </c>
       <c r="AL309" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="AM309">
         <v>1</v>
@@ -34194,7 +34197,7 @@
         <v>352</v>
       </c>
       <c r="AL310" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="AM310">
         <v>1</v>
@@ -34298,7 +34301,7 @@
         <v>353</v>
       </c>
       <c r="AL311" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="AM311">
         <v>1</v>
@@ -34399,10 +34402,10 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="AK312">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="AL312" t="s">
-        <v>1427</v>
+        <v>1562</v>
       </c>
       <c r="AM312">
         <v>1</v>
@@ -34500,7 +34503,7 @@
         <v>365</v>
       </c>
       <c r="AL313" t="s">
-        <v>1404</v>
+        <v>1427</v>
       </c>
       <c r="AM313">
         <v>1</v>
@@ -34598,10 +34601,10 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="AK314">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AL314" t="s">
-        <v>1425</v>
+        <v>1404</v>
       </c>
       <c r="AM314">
         <v>1</v>
@@ -34696,10 +34699,10 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="AK315">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AL315" t="s">
-        <v>1473</v>
+        <v>1425</v>
       </c>
       <c r="AM315">
         <v>1</v>
@@ -34800,7 +34803,7 @@
         <v>370</v>
       </c>
       <c r="AL316" t="s">
-        <v>1392</v>
+        <v>1473</v>
       </c>
       <c r="AM316">
         <v>1</v>
@@ -34901,7 +34904,7 @@
         <v>371</v>
       </c>
       <c r="AL317" t="s">
-        <v>1402</v>
+        <v>1392</v>
       </c>
       <c r="AM317">
         <v>1</v>
@@ -34999,7 +35002,7 @@
         <v>372</v>
       </c>
       <c r="AL318" t="s">
-        <v>1384</v>
+        <v>1402</v>
       </c>
       <c r="AM318">
         <v>1</v>
@@ -35098,7 +35101,7 @@
         <v>373</v>
       </c>
       <c r="AL319" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="AM319">
         <v>1</v>
@@ -35197,7 +35200,7 @@
         <v>374</v>
       </c>
       <c r="AL320" t="s">
-        <v>1420</v>
+        <v>1386</v>
       </c>
       <c r="AM320">
         <v>1</v>
@@ -35293,7 +35296,7 @@
         <v>375</v>
       </c>
       <c r="AL321" t="s">
-        <v>1393</v>
+        <v>1420</v>
       </c>
       <c r="AM321">
         <v>1</v>
@@ -35392,7 +35395,7 @@
         <v>376</v>
       </c>
       <c r="AL322" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="AM322">
         <v>1</v>
@@ -35488,7 +35491,7 @@
         <v>377</v>
       </c>
       <c r="AL323" t="s">
-        <v>1421</v>
+        <v>1389</v>
       </c>
       <c r="AM323">
         <v>1</v>
@@ -35587,7 +35590,7 @@
         <v>378</v>
       </c>
       <c r="AL324" t="s">
-        <v>1376</v>
+        <v>1421</v>
       </c>
       <c r="AM324">
         <v>1</v>
@@ -35683,7 +35686,7 @@
         <v>379</v>
       </c>
       <c r="AL325" t="s">
-        <v>1391</v>
+        <v>1376</v>
       </c>
       <c r="AM325">
         <v>1</v>
@@ -35753,7 +35756,7 @@
         <v>380</v>
       </c>
       <c r="AL326" t="s">
-        <v>1382</v>
+        <v>1391</v>
       </c>
       <c r="AM326">
         <v>1</v>
@@ -35826,7 +35829,7 @@
         <v>381</v>
       </c>
       <c r="AL327" t="s">
-        <v>1429</v>
+        <v>1382</v>
       </c>
       <c r="AM327">
         <v>1</v>
@@ -35896,7 +35899,7 @@
         <v>1002</v>
       </c>
       <c r="AL328" t="s">
-        <v>1380</v>
+        <v>1429</v>
       </c>
       <c r="AM328">
         <v>1</v>
@@ -35961,7 +35964,7 @@
         <v>1022</v>
       </c>
       <c r="AL329" t="s">
-        <v>1409</v>
+        <v>1380</v>
       </c>
       <c r="AM329">
         <v>1</v>
@@ -36026,7 +36029,7 @@
         <v>1022</v>
       </c>
       <c r="AL330" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="AM330">
         <v>1</v>
@@ -36091,7 +36094,7 @@
         <v>1002</v>
       </c>
       <c r="AL331" t="s">
-        <v>1390</v>
+        <v>1411</v>
       </c>
       <c r="AM331">
         <v>1</v>
@@ -36158,14 +36161,11 @@
       <c r="X332" s="24" t="s">
         <v>1023</v>
       </c>
-      <c r="AK332">
-        <v>9</v>
-      </c>
       <c r="AL332" t="s">
-        <v>1521</v>
+        <v>1390</v>
       </c>
       <c r="AM332">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="333" spans="1:39" x14ac:dyDescent="0.25">
@@ -36230,10 +36230,10 @@
         <v>1023</v>
       </c>
       <c r="AK333">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="AL333" t="s">
-        <v>1217</v>
+        <v>1521</v>
       </c>
       <c r="AM333">
         <v>2</v>
@@ -36295,10 +36295,10 @@
         <v>1022</v>
       </c>
       <c r="AK334">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AL334" t="s">
-        <v>1239</v>
+        <v>1217</v>
       </c>
       <c r="AM334">
         <v>2</v>
@@ -36359,10 +36359,10 @@
         <v>40</v>
       </c>
       <c r="AK335">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="AL335" t="s">
-        <v>1359</v>
+        <v>1239</v>
       </c>
       <c r="AM335">
         <v>2</v>
@@ -36429,10 +36429,10 @@
         <v>1331</v>
       </c>
       <c r="AK336">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AL336" t="s">
-        <v>1422</v>
+        <v>1359</v>
       </c>
       <c r="AM336">
         <v>2</v>
@@ -36499,10 +36499,10 @@
         <v>1336</v>
       </c>
       <c r="AK337">
-        <v>305</v>
+        <v>69</v>
       </c>
       <c r="AL337" t="s">
-        <v>1273</v>
+        <v>1422</v>
       </c>
       <c r="AM337">
         <v>2</v>
@@ -36572,10 +36572,10 @@
         <v>1334</v>
       </c>
       <c r="AK338">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AL338" t="s">
-        <v>1265</v>
+        <v>1273</v>
       </c>
       <c r="AM338">
         <v>2</v>
@@ -36645,10 +36645,10 @@
         <v>1340</v>
       </c>
       <c r="AK339">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AL339" t="s">
-        <v>1277</v>
+        <v>1265</v>
       </c>
       <c r="AM339">
         <v>2</v>
@@ -36727,13 +36727,13 @@
         <v>1335</v>
       </c>
       <c r="AK340">
-        <v>33</v>
+        <v>312</v>
       </c>
       <c r="AL340" t="s">
-        <v>1226</v>
+        <v>1277</v>
       </c>
       <c r="AM340">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="341" spans="1:39" x14ac:dyDescent="0.25">
@@ -36803,10 +36803,10 @@
         <v>1516</v>
       </c>
       <c r="AK341">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="AL341" t="s">
-        <v>798</v>
+        <v>1226</v>
       </c>
       <c r="AM341">
         <v>3</v>
@@ -36873,10 +36873,10 @@
         <v>0</v>
       </c>
       <c r="AK342">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AL342" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="AM342">
         <v>3</v>
@@ -36955,10 +36955,10 @@
         <v>1650</v>
       </c>
       <c r="AK343">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL343" t="s">
-        <v>1362</v>
+        <v>799</v>
       </c>
       <c r="AM343">
         <v>3</v>
@@ -37025,10 +37025,10 @@
         <v>4</v>
       </c>
       <c r="AK344">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AL344" t="s">
-        <v>1356</v>
+        <v>1362</v>
       </c>
       <c r="AM344">
         <v>3</v>
@@ -37093,10 +37093,10 @@
         <v>20</v>
       </c>
       <c r="AK345">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="AL345" t="s">
-        <v>1260</v>
+        <v>1356</v>
       </c>
       <c r="AM345">
         <v>3</v>
@@ -37154,10 +37154,10 @@
         <v>Soldrota-E</v>
       </c>
       <c r="AK346">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AL346" t="s">
-        <v>1412</v>
+        <v>1260</v>
       </c>
       <c r="AM346">
         <v>3</v>
@@ -37216,10 +37216,10 @@
         <v>35</v>
       </c>
       <c r="AK347">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AL347" t="s">
-        <v>1227</v>
+        <v>1412</v>
       </c>
       <c r="AM347">
         <v>3</v>
@@ -37278,10 +37278,10 @@
         <v>55</v>
       </c>
       <c r="AK348">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AL348" t="s">
-        <v>1282</v>
+        <v>1227</v>
       </c>
       <c r="AM348">
         <v>3</v>
@@ -37337,10 +37337,10 @@
         <v>Blastflames-E</v>
       </c>
       <c r="AK349">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AL349" t="s">
-        <v>1249</v>
+        <v>1282</v>
       </c>
       <c r="AM349">
         <v>3</v>
@@ -37399,10 +37399,10 @@
         <v>22</v>
       </c>
       <c r="AK350">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AL350" t="s">
-        <v>1276</v>
+        <v>1249</v>
       </c>
       <c r="AM350">
         <v>3</v>
@@ -37461,10 +37461,10 @@
         <v>796</v>
       </c>
       <c r="AK351">
-        <v>302</v>
+        <v>82</v>
       </c>
       <c r="AL351" t="s">
-        <v>1229</v>
+        <v>1276</v>
       </c>
       <c r="AM351">
         <v>3</v>
@@ -37523,7 +37523,7 @@
         <v>303</v>
       </c>
       <c r="AL352" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="AM352">
         <v>3</v>
@@ -37585,7 +37585,7 @@
         <v>304</v>
       </c>
       <c r="AL353" t="s">
-        <v>1264</v>
+        <v>1230</v>
       </c>
       <c r="AM353">
         <v>3</v>
@@ -37644,13 +37644,13 @@
         <v>20</v>
       </c>
       <c r="AK354">
-        <v>2</v>
+        <v>305</v>
       </c>
       <c r="AL354" t="s">
-        <v>1244</v>
+        <v>1264</v>
       </c>
       <c r="AM354">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="355" spans="1:39" x14ac:dyDescent="0.25">
@@ -37706,10 +37706,10 @@
         <v>Gyarados-E</v>
       </c>
       <c r="AK355">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="AL355" t="s">
-        <v>1220</v>
+        <v>1244</v>
       </c>
       <c r="AM355">
         <v>4</v>
@@ -37767,10 +37767,10 @@
         <v>Shockfang</v>
       </c>
       <c r="AK356">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="AL356" t="s">
-        <v>1237</v>
+        <v>1220</v>
       </c>
       <c r="AM356">
         <v>4</v>
@@ -37831,10 +37831,10 @@
         <v>40</v>
       </c>
       <c r="AK357">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="AL357" t="s">
-        <v>1375</v>
+        <v>1237</v>
       </c>
       <c r="AM357">
         <v>4</v>
@@ -37892,10 +37892,10 @@
         <v>Nightrex</v>
       </c>
       <c r="AK358">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AL358" t="s">
-        <v>1215</v>
+        <v>1375</v>
       </c>
       <c r="AM358">
         <v>4</v>
@@ -37956,10 +37956,10 @@
         <v>40</v>
       </c>
       <c r="AK359">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AL359" t="s">
-        <v>1223</v>
+        <v>1215</v>
       </c>
       <c r="AM359">
         <v>4</v>
@@ -38015,10 +38015,10 @@
         <v>Durfish-S</v>
       </c>
       <c r="AK360">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AL360" t="s">
-        <v>1248</v>
+        <v>1223</v>
       </c>
       <c r="AM360">
         <v>4</v>
@@ -38077,10 +38077,10 @@
         <v>794</v>
       </c>
       <c r="AK361">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL361" t="s">
-        <v>1355</v>
+        <v>1248</v>
       </c>
       <c r="AM361">
         <v>4</v>
@@ -38135,10 +38135,10 @@
         <v>Wormite-S</v>
       </c>
       <c r="AK362">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AL362" t="s">
-        <v>1361</v>
+        <v>1355</v>
       </c>
       <c r="AM362">
         <v>4</v>
@@ -38196,10 +38196,10 @@
         <v>20</v>
       </c>
       <c r="AK363">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AL363" t="s">
-        <v>1350</v>
+        <v>1361</v>
       </c>
       <c r="AM363">
         <v>4</v>
@@ -38256,8 +38256,11 @@
       <c r="R364">
         <v>45</v>
       </c>
+      <c r="AK364">
+        <v>75</v>
+      </c>
       <c r="AL364" t="s">
-        <v>1423</v>
+        <v>1350</v>
       </c>
       <c r="AM364">
         <v>4</v>
@@ -38311,14 +38314,11 @@
         <f t="shared" si="20"/>
         <v>Cluuz-S</v>
       </c>
-      <c r="AK365">
-        <v>1</v>
-      </c>
       <c r="AL365" t="s">
-        <v>1267</v>
+        <v>1423</v>
       </c>
       <c r="AM365">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="366" spans="1:39" x14ac:dyDescent="0.25">
@@ -38373,10 +38373,10 @@
         <v>794</v>
       </c>
       <c r="AK366">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="AL366" t="s">
-        <v>1263</v>
+        <v>1267</v>
       </c>
       <c r="AM366">
         <v>5</v>
@@ -38434,10 +38434,10 @@
         <v>788</v>
       </c>
       <c r="AK367">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="AL367" t="s">
-        <v>1373</v>
+        <v>1263</v>
       </c>
       <c r="AM367">
         <v>5</v>
@@ -38498,10 +38498,10 @@
         <v>16</v>
       </c>
       <c r="AK368">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL368" t="s">
-        <v>1231</v>
+        <v>1373</v>
       </c>
       <c r="AM368">
         <v>5</v>
@@ -38562,10 +38562,10 @@
         <v>36</v>
       </c>
       <c r="AK369">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="AL369" t="s">
-        <v>1225</v>
+        <v>1231</v>
       </c>
       <c r="AM369">
         <v>5</v>
@@ -38623,10 +38623,10 @@
         <v>Pyrator-S</v>
       </c>
       <c r="AK370">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="AL370" t="s">
-        <v>1352</v>
+        <v>1225</v>
       </c>
       <c r="AM370">
         <v>5</v>
@@ -38687,10 +38687,10 @@
         <v>32</v>
       </c>
       <c r="AK371">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="AL371" t="s">
-        <v>1488</v>
+        <v>1352</v>
       </c>
       <c r="AM371">
         <v>5</v>
@@ -38748,10 +38748,10 @@
         <v>Arbok-S</v>
       </c>
       <c r="AK372">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AL372" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="AM372">
         <v>5</v>
@@ -38807,10 +38807,10 @@
         <v>862</v>
       </c>
       <c r="AK373">
-        <v>310</v>
+        <v>163</v>
       </c>
       <c r="AL373" t="s">
-        <v>1261</v>
+        <v>1489</v>
       </c>
       <c r="AM373">
         <v>5</v>
@@ -38865,8 +38865,11 @@
       <c r="R374" t="s">
         <v>866</v>
       </c>
+      <c r="AK374">
+        <v>311</v>
+      </c>
       <c r="AL374" t="s">
-        <v>1424</v>
+        <v>1261</v>
       </c>
       <c r="AM374">
         <v>5</v>
@@ -38921,14 +38924,11 @@
       <c r="R375" t="s">
         <v>863</v>
       </c>
-      <c r="AK375">
-        <v>30</v>
-      </c>
       <c r="AL375" t="s">
-        <v>1241</v>
+        <v>1424</v>
       </c>
       <c r="AM375">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="376" spans="1:40" x14ac:dyDescent="0.25">
@@ -38981,10 +38981,10 @@
         <v>819</v>
       </c>
       <c r="AK376">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="AL376" t="s">
-        <v>1251</v>
+        <v>1241</v>
       </c>
       <c r="AM376">
         <v>6</v>
@@ -39040,10 +39040,10 @@
         <v>863</v>
       </c>
       <c r="AK377">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AL377" t="s">
-        <v>1234</v>
+        <v>1251</v>
       </c>
       <c r="AM377">
         <v>6</v>
@@ -39099,10 +39099,10 @@
         <v>849</v>
       </c>
       <c r="AK378">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AL378" t="s">
-        <v>1247</v>
+        <v>1234</v>
       </c>
       <c r="AM378">
         <v>6</v>
@@ -39158,10 +39158,10 @@
         <v>851</v>
       </c>
       <c r="AK379">
-        <v>172</v>
+        <v>56</v>
       </c>
       <c r="AL379" t="s">
-        <v>907</v>
+        <v>1247</v>
       </c>
       <c r="AM379">
         <v>6</v>
@@ -39217,10 +39217,10 @@
         <v>864</v>
       </c>
       <c r="AK380">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AL380" t="s">
-        <v>1019</v>
+        <v>907</v>
       </c>
       <c r="AM380">
         <v>6</v>
@@ -39276,10 +39276,10 @@
         <v>1092</v>
       </c>
       <c r="AK381">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AL381" t="s">
-        <v>1497</v>
+        <v>1019</v>
       </c>
       <c r="AM381">
         <v>6</v>
@@ -39328,16 +39328,13 @@
         <v>Kissyfishy-D</v>
       </c>
       <c r="AK382">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="AL382" t="s">
-        <v>1539</v>
+        <v>1497</v>
       </c>
       <c r="AM382">
         <v>6</v>
-      </c>
-      <c r="AN382" t="s">
-        <v>1563</v>
       </c>
     </row>
     <row r="383" spans="1:40" x14ac:dyDescent="0.25">
@@ -39385,10 +39382,10 @@
         <v>623</v>
       </c>
       <c r="AK383">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AL383" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="AM383">
         <v>6</v>
@@ -39442,10 +39439,10 @@
         <v>623</v>
       </c>
       <c r="AK384">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AL384" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="AM384">
         <v>6</v>
@@ -39499,10 +39496,10 @@
         <v>623</v>
       </c>
       <c r="AK385">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AL385" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="AM385">
         <v>6</v>
@@ -39547,13 +39544,16 @@
         <v>350</v>
       </c>
       <c r="AK386">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="AL386" t="s">
-        <v>1491</v>
+        <v>1542</v>
       </c>
       <c r="AM386">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="AN386" t="s">
+        <v>1563</v>
       </c>
     </row>
     <row r="387" spans="1:40" x14ac:dyDescent="0.25">
@@ -39592,10 +39592,10 @@
         <v>525</v>
       </c>
       <c r="AK387">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AL387" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="AM387">
         <v>7</v>
@@ -39637,10 +39637,10 @@
         <v>310</v>
       </c>
       <c r="AK388">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AL388" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="AM388">
         <v>7</v>
@@ -39682,10 +39682,10 @@
         <v>400</v>
       </c>
       <c r="AK389">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AL389" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="AM389">
         <v>7</v>
@@ -39727,10 +39727,10 @@
         <v>500</v>
       </c>
       <c r="AK390">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="AL390" t="s">
-        <v>1498</v>
+        <v>1494</v>
       </c>
       <c r="AM390">
         <v>7</v>
@@ -39772,13 +39772,13 @@
         <v>500</v>
       </c>
       <c r="AK391">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="AL391" t="s">
-        <v>1280</v>
+        <v>1498</v>
       </c>
       <c r="AM391">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="392" spans="1:40" x14ac:dyDescent="0.25">
@@ -39817,10 +39817,10 @@
         <v>430</v>
       </c>
       <c r="AK392">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="AL392" t="s">
-        <v>1235</v>
+        <v>1280</v>
       </c>
       <c r="AM392">
         <v>8</v>
@@ -39862,10 +39862,10 @@
         <v>510</v>
       </c>
       <c r="AK393">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="AL393" t="s">
-        <v>1495</v>
+        <v>1235</v>
       </c>
       <c r="AM393">
         <v>8</v>
@@ -39907,10 +39907,10 @@
         <v>510</v>
       </c>
       <c r="AK394">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="AL394" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
       <c r="AM394">
         <v>8</v>
@@ -39952,16 +39952,13 @@
         <v>510</v>
       </c>
       <c r="AK395">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AL395" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="AM395">
         <v>8</v>
-      </c>
-      <c r="AN395" t="s">
-        <v>1563</v>
       </c>
     </row>
     <row r="396" spans="1:40" x14ac:dyDescent="0.25">
@@ -40000,13 +39997,16 @@
         <v>290</v>
       </c>
       <c r="AK396">
-        <v>36</v>
+        <v>181</v>
       </c>
       <c r="AL396" t="s">
-        <v>1240</v>
+        <v>1500</v>
       </c>
       <c r="AM396">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="AN396" t="s">
+        <v>1563</v>
       </c>
     </row>
     <row r="397" spans="1:40" x14ac:dyDescent="0.25">
@@ -40045,10 +40045,10 @@
         <v>370</v>
       </c>
       <c r="AK397">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="AL397" t="s">
-        <v>1214</v>
+        <v>1240</v>
       </c>
       <c r="AM397">
         <v>9</v>
@@ -40090,10 +40090,10 @@
         <v>490</v>
       </c>
       <c r="AK398">
-        <v>164</v>
+        <v>60</v>
       </c>
       <c r="AL398" t="s">
-        <v>901</v>
+        <v>1214</v>
       </c>
       <c r="AM398">
         <v>9</v>
@@ -40135,10 +40135,10 @@
         <v>290</v>
       </c>
       <c r="AK399">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AL399" t="s">
-        <v>908</v>
+        <v>901</v>
       </c>
       <c r="AM399">
         <v>9</v>
@@ -40180,10 +40180,10 @@
         <v>370</v>
       </c>
       <c r="AK400">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AL400" t="s">
-        <v>1258</v>
+        <v>908</v>
       </c>
       <c r="AM400">
         <v>9</v>
@@ -40225,10 +40225,10 @@
         <v>490</v>
       </c>
       <c r="AK401">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AL401" t="s">
-        <v>1490</v>
+        <v>1258</v>
       </c>
       <c r="AM401">
         <v>9</v>
@@ -40270,10 +40270,10 @@
         <v>458</v>
       </c>
       <c r="AK402">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="AL402" t="s">
-        <v>1017</v>
+        <v>1490</v>
       </c>
       <c r="AM402">
         <v>9</v>
@@ -40315,10 +40315,10 @@
         <v>535</v>
       </c>
       <c r="AK403">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AL403" t="s">
-        <v>1496</v>
+        <v>1017</v>
       </c>
       <c r="AM403">
         <v>9</v>
@@ -40360,13 +40360,13 @@
         <v>312</v>
       </c>
       <c r="AK404">
-        <v>26</v>
+        <v>177</v>
       </c>
       <c r="AL404" t="s">
-        <v>1268</v>
+        <v>1496</v>
       </c>
       <c r="AM404">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="405" spans="1:39" x14ac:dyDescent="0.25">
@@ -40405,10 +40405,10 @@
         <v>487</v>
       </c>
       <c r="AK405">
-        <v>161</v>
+        <v>26</v>
       </c>
       <c r="AL405" t="s">
-        <v>1216</v>
+        <v>1268</v>
       </c>
       <c r="AM405">
         <v>10</v>
@@ -40450,10 +40450,10 @@
         <v>332</v>
       </c>
       <c r="AK406">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="AL406" t="s">
-        <v>1018</v>
+        <v>1216</v>
       </c>
       <c r="AM406">
         <v>10</v>
@@ -40495,13 +40495,13 @@
         <v>497</v>
       </c>
       <c r="AK407">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="AL407" t="s">
-        <v>1256</v>
+        <v>1018</v>
       </c>
       <c r="AM407">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="408" spans="1:39" x14ac:dyDescent="0.25">
@@ -40540,10 +40540,10 @@
         <v>410</v>
       </c>
       <c r="AK408">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="AL408" t="s">
-        <v>1269</v>
+        <v>1256</v>
       </c>
       <c r="AM408">
         <v>12</v>
@@ -40584,8 +40584,11 @@
       <c r="K409">
         <v>570</v>
       </c>
+      <c r="AK409">
+        <v>44</v>
+      </c>
       <c r="AL409" t="s">
-        <v>1342</v>
+        <v>1269</v>
       </c>
       <c r="AM409">
         <v>12</v>
@@ -40632,14 +40635,11 @@
       <c r="N410" t="s">
         <v>1191</v>
       </c>
-      <c r="AK410">
-        <v>3</v>
-      </c>
       <c r="AL410" t="s">
-        <v>1327</v>
+        <v>1342</v>
       </c>
       <c r="AM410">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="411" spans="1:39" x14ac:dyDescent="0.25">
@@ -40684,10 +40684,10 @@
         <v>1191</v>
       </c>
       <c r="AK411">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="AL411" t="s">
-        <v>1257</v>
+        <v>1327</v>
       </c>
       <c r="AM411">
         <v>13</v>
@@ -40728,11 +40728,14 @@
       <c r="K412">
         <v>335</v>
       </c>
+      <c r="AK412">
+        <v>39</v>
+      </c>
       <c r="AL412" t="s">
-        <v>1371</v>
+        <v>1257</v>
       </c>
       <c r="AM412">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="413" spans="1:39" x14ac:dyDescent="0.25">
@@ -40771,7 +40774,7 @@
         <v>485</v>
       </c>
       <c r="AL413" t="s">
-        <v>1343</v>
+        <v>1371</v>
       </c>
       <c r="AM413">
         <v>14</v>
@@ -40812,14 +40815,11 @@
       <c r="K414">
         <v>195</v>
       </c>
-      <c r="AK414">
-        <v>42</v>
-      </c>
       <c r="AL414" t="s">
-        <v>1255</v>
+        <v>1343</v>
       </c>
       <c r="AM414">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="415" spans="1:39" x14ac:dyDescent="0.25">
@@ -40858,13 +40858,13 @@
         <v>205</v>
       </c>
       <c r="AK415">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AL415" t="s">
-        <v>1243</v>
+        <v>1255</v>
       </c>
       <c r="AM415">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="416" spans="1:39" x14ac:dyDescent="0.25">
@@ -40902,8 +40902,11 @@
       <c r="K416">
         <v>400</v>
       </c>
+      <c r="AK416">
+        <v>49</v>
+      </c>
       <c r="AL416" t="s">
-        <v>1413</v>
+        <v>1243</v>
       </c>
       <c r="AM416">
         <v>17</v>
@@ -40944,14 +40947,11 @@
       <c r="K417">
         <v>210</v>
       </c>
-      <c r="AK417">
-        <v>160</v>
-      </c>
       <c r="AL417" t="s">
-        <v>894</v>
+        <v>1413</v>
       </c>
       <c r="AM417">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="418" spans="1:39" x14ac:dyDescent="0.25">
@@ -40993,13 +40993,13 @@
         <v>1172</v>
       </c>
       <c r="AK418">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="AL418" t="s">
-        <v>1246</v>
+        <v>894</v>
       </c>
       <c r="AM418">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="419" spans="1:39" x14ac:dyDescent="0.25">
@@ -41038,10 +41038,10 @@
         <v>300</v>
       </c>
       <c r="AK419">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="AL419" t="s">
-        <v>1275</v>
+        <v>1246</v>
       </c>
       <c r="AM419">
         <v>19</v>
@@ -41083,10 +41083,10 @@
         <v>500</v>
       </c>
       <c r="AK420">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="AL420" t="s">
-        <v>1270</v>
+        <v>1275</v>
       </c>
       <c r="AM420">
         <v>19</v>
@@ -41128,10 +41128,10 @@
         <v>300</v>
       </c>
       <c r="AK421">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="AL421" t="s">
-        <v>1236</v>
+        <v>1270</v>
       </c>
       <c r="AM421">
         <v>19</v>
@@ -41176,13 +41176,13 @@
         <v>1172</v>
       </c>
       <c r="AK422">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="AL422" t="s">
-        <v>1365</v>
+        <v>1236</v>
       </c>
       <c r="AM422">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="423" spans="1:39" x14ac:dyDescent="0.25">
@@ -41230,13 +41230,13 @@
         <v>1186</v>
       </c>
       <c r="AK423">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="AL423" t="s">
-        <v>1274</v>
+        <v>1365</v>
       </c>
       <c r="AM423">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="424" spans="1:39" x14ac:dyDescent="0.25">
@@ -41284,13 +41284,13 @@
         <v>1186</v>
       </c>
       <c r="AK424">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="AL424" t="s">
-        <v>1224</v>
+        <v>1274</v>
       </c>
       <c r="AM424">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="425" spans="1:39" x14ac:dyDescent="0.25">
@@ -41341,13 +41341,13 @@
         <v>1187</v>
       </c>
       <c r="AK425">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AL425" t="s">
-        <v>1272</v>
+        <v>1224</v>
       </c>
       <c r="AM425">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="426" spans="1:39" x14ac:dyDescent="0.25">
@@ -41394,11 +41394,14 @@
       <c r="N426" t="s">
         <v>1188</v>
       </c>
+      <c r="AK426">
+        <v>40</v>
+      </c>
       <c r="AL426" t="s">
-        <v>1369</v>
+        <v>1272</v>
       </c>
       <c r="AM426">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="427" spans="1:39" x14ac:dyDescent="0.25">
@@ -41444,6 +41447,12 @@
       </c>
       <c r="N427" t="s">
         <v>1188</v>
+      </c>
+      <c r="AL427" t="s">
+        <v>1369</v>
+      </c>
+      <c r="AM427">
+        <v>47</v>
       </c>
     </row>
     <row r="428" spans="1:39" x14ac:dyDescent="0.25">

</xml_diff>